<commit_message>
13% correct with number non fancy way
</commit_message>
<xml_diff>
--- a/baby.xlsx
+++ b/baby.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Review-Tagging-Process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CA245E-363D-453D-BB6A-9076E7398DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B38F2-7721-4816-B963-B7FD778179A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2730" windowWidth="14400" windowHeight="7350" xr2:uid="{FD4C3268-3A96-4A63-A994-F8CB3D1D7B4B}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7350" xr2:uid="{FD4C3268-3A96-4A63-A994-F8CB3D1D7B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
-  <si>
-    <t>Good Dog</t>
-  </si>
-  <si>
-    <t>Bad Cat</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
   <si>
     <t>one</t>
   </si>
@@ -49,13 +43,19 @@
     <t xml:space="preserve">two </t>
   </si>
   <si>
-    <t>Good Bad</t>
-  </si>
-  <si>
-    <t>Three</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good </t>
+    <t>two</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>john</t>
   </si>
 </sst>
 </file>
@@ -407,63 +407,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A266878A-457B-4554-B7C6-A3923227F3FE}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+      <c r="B18" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>